<commit_message>
Choix de catégorie quand on veut jouer avec le passage de paramètre d'un formulaire à l'autre
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeBord-Jeremy.xlsx
+++ b/Documentation/JournalDeBord-Jeremy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>date</t>
   </si>
@@ -81,6 +81,27 @@
   </si>
   <si>
     <t>gestion sur le projet (issues pour sprint 2), un peu de documentation</t>
+  </si>
+  <si>
+    <t>----</t>
+  </si>
+  <si>
+    <t>Interface graphique du jeu</t>
+  </si>
+  <si>
+    <t>Travail fourni durant les vacances</t>
+  </si>
+  <si>
+    <t>Jsuite au commit de mon ordinateur perso j'ai remarqué qu'il y a des fichiers supplémentaire qui sont visible dans le commit qui avant n'apparaissaient pas (Pendu\.vs\Pendu\v15)</t>
+  </si>
+  <si>
+    <t>Mise en commun du projet avec correction de merge, Création dynamique des boutons de categorie de mot lors du jeu, passage au jeu</t>
+  </si>
+  <si>
+    <t>J'ai eu un problème de creation de boutton dynamique avec une liste et passer un paramètre d'un formulaire à un autre</t>
+  </si>
+  <si>
+    <t>Mme Andolfatto m'a donné un coup de main pour la liste et M. Ithurbide m'a montré le constructeur principale et le simple sans paramètre</t>
   </si>
 </sst>
 </file>
@@ -340,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -386,7 +407,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -413,14 +443,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -811,7 +835,7 @@
   <dimension ref="A1:AB80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -826,12 +850,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -858,16 +882,16 @@
       <c r="AB1" s="1"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="26" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -890,14 +914,14 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -981,14 +1005,14 @@
     </row>
     <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="24"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1011,14 +1035,14 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="25"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1041,7 +1065,7 @@
     </row>
     <row r="8" spans="1:28" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="19"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1060,7 +1084,7 @@
       <c r="H8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="22"/>
+      <c r="I8" s="25"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1083,7 +1107,7 @@
     </row>
     <row r="9" spans="1:28" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="19"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="7">
         <v>43438</v>
       </c>
@@ -1100,7 +1124,7 @@
       <c r="H9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="22"/>
+      <c r="I9" s="25"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1123,7 +1147,7 @@
     </row>
     <row r="10" spans="1:28" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="19"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="10">
         <v>43441</v>
       </c>
@@ -1136,7 +1160,7 @@
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="22"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1159,7 +1183,7 @@
     </row>
     <row r="11" spans="1:28" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="19"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="10">
         <v>43445</v>
       </c>
@@ -1178,7 +1202,7 @@
       <c r="H11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="22"/>
+      <c r="I11" s="25"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1201,14 +1225,22 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="10">
+        <v>43471</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="G12" s="12"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="22"/>
+      <c r="I12" s="25"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1229,16 +1261,28 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="10">
+        <v>43473</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="25"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1261,14 +1305,14 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="19"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="22"/>
+      <c r="I14" s="25"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1291,14 +1335,14 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="19"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="12"/>
       <c r="H15" s="13"/>
-      <c r="I15" s="22"/>
+      <c r="I15" s="25"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1321,14 +1365,14 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="19"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="13"/>
-      <c r="I16" s="22"/>
+      <c r="I16" s="25"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1351,14 +1395,14 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="19"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="13"/>
-      <c r="I17" s="22"/>
+      <c r="I17" s="25"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1381,14 +1425,14 @@
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="19"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="22"/>
+      <c r="I18" s="25"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1411,14 +1455,14 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="19"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="10"/>
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="22"/>
+      <c r="I19" s="25"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1441,14 +1485,14 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="19"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="14"/>
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="22"/>
+      <c r="I20" s="25"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1471,14 +1515,14 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="19"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="14"/>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="22"/>
+      <c r="I21" s="25"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1501,14 +1545,14 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="19"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="14"/>
       <c r="D22" s="11"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="22"/>
+      <c r="I22" s="25"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1531,14 +1575,14 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
-      <c r="B23" s="19"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="14"/>
       <c r="D23" s="11"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
       <c r="H23" s="13"/>
-      <c r="I23" s="22"/>
+      <c r="I23" s="25"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1561,14 +1605,14 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="19"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="14"/>
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="22"/>
+      <c r="I24" s="25"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1591,14 +1635,14 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="19"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="14"/>
       <c r="D25" s="11"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="13"/>
-      <c r="I25" s="22"/>
+      <c r="I25" s="25"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1621,14 +1665,14 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="B26" s="19"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="14"/>
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="13"/>
-      <c r="I26" s="22"/>
+      <c r="I26" s="25"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1651,14 +1695,14 @@
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="19"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="14"/>
       <c r="D27" s="11"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="22"/>
+      <c r="I27" s="25"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1681,14 +1725,14 @@
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="19"/>
+      <c r="B28" s="22"/>
       <c r="C28" s="14"/>
       <c r="D28" s="11"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="13"/>
-      <c r="I28" s="22"/>
+      <c r="I28" s="25"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1711,14 +1755,14 @@
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="19"/>
+      <c r="B29" s="22"/>
       <c r="C29" s="14"/>
       <c r="D29" s="11"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
       <c r="H29" s="13"/>
-      <c r="I29" s="22"/>
+      <c r="I29" s="25"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1741,14 +1785,14 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="B30" s="19"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="14"/>
       <c r="D30" s="11"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="13"/>
-      <c r="I30" s="22"/>
+      <c r="I30" s="25"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1771,14 +1815,14 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
-      <c r="B31" s="19"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="14"/>
       <c r="D31" s="11"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="13"/>
-      <c r="I31" s="22"/>
+      <c r="I31" s="25"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1801,14 +1845,14 @@
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="B32" s="19"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="14"/>
       <c r="D32" s="11"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
       <c r="H32" s="13"/>
-      <c r="I32" s="22"/>
+      <c r="I32" s="25"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1831,14 +1875,14 @@
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="19"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="14"/>
       <c r="D33" s="11"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
       <c r="H33" s="13"/>
-      <c r="I33" s="22"/>
+      <c r="I33" s="25"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1861,14 +1905,14 @@
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="19"/>
+      <c r="B34" s="22"/>
       <c r="C34" s="14"/>
       <c r="D34" s="11"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
       <c r="H34" s="13"/>
-      <c r="I34" s="22"/>
+      <c r="I34" s="25"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -1891,14 +1935,14 @@
     </row>
     <row r="35" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="26"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>

</xml_diff>